<commit_message>
Trying to make the whole thing lighter to run
With 10,1000 simulations it causes memory crashes...
</commit_message>
<xml_diff>
--- a/output/sites/table_summary_model_parameters.xlsx
+++ b/output/sites/table_summary_model_parameters.xlsx
@@ -446,22 +446,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>662</v>
+        <v>500</v>
       </c>
       <c r="C2" t="n">
-        <v>665</v>
+        <v>508</v>
       </c>
       <c r="D2" t="n">
-        <v>728</v>
+        <v>669</v>
       </c>
       <c r="E2" t="n">
-        <v>726</v>
+        <v>668</v>
       </c>
       <c r="F2" t="n">
-        <v>790</v>
+        <v>829</v>
       </c>
       <c r="G2" t="n">
-        <v>794</v>
+        <v>838</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -472,22 +472,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>913</v>
+        <v>942</v>
       </c>
       <c r="C3" t="n">
-        <v>919</v>
+        <v>948</v>
       </c>
       <c r="D3" t="n">
-        <v>1008</v>
+        <v>1054</v>
       </c>
       <c r="E3" t="n">
-        <v>1006</v>
+        <v>1055</v>
       </c>
       <c r="F3" t="n">
-        <v>1091</v>
+        <v>1158</v>
       </c>
       <c r="G3" t="n">
-        <v>1095</v>
+        <v>1163</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
@@ -499,7 +499,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>20.68</v>
+        <v>20.69</v>
       </c>
       <c r="D4" t="n">
         <v>27.63</v>
@@ -508,7 +508,7 @@
         <v>27.42</v>
       </c>
       <c r="F4" t="n">
-        <v>35.96</v>
+        <v>35.97</v>
       </c>
       <c r="G4" t="n">
         <v>38</v>
@@ -523,7 +523,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="n">
-        <v>20.68</v>
+        <v>20.69</v>
       </c>
       <c r="D5" t="n">
         <v>27.63</v>
@@ -532,7 +532,7 @@
         <v>27.42</v>
       </c>
       <c r="F5" t="n">
-        <v>35.98</v>
+        <v>35.96</v>
       </c>
       <c r="G5" t="n">
         <v>38</v>
@@ -544,7 +544,7 @@
     <row r="6">
       <c r="A6"/>
       <c r="B6" t="n">
-        <v>2.85</v>
+        <v>2.79</v>
       </c>
       <c r="C6" t="n">
         <v>3.1</v>
@@ -559,7 +559,7 @@
         <v>3.5</v>
       </c>
       <c r="G6" t="n">
-        <v>3.77</v>
+        <v>3.79</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -568,7 +568,7 @@
     <row r="7">
       <c r="A7"/>
       <c r="B7" t="n">
-        <v>2.82</v>
+        <v>2.8</v>
       </c>
       <c r="C7" t="n">
         <v>3.1</v>
@@ -583,7 +583,7 @@
         <v>3.5</v>
       </c>
       <c r="G7" t="n">
-        <v>3.76</v>
+        <v>3.83</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -607,7 +607,7 @@
         <v>5.29</v>
       </c>
       <c r="G8" t="n">
-        <v>6.22</v>
+        <v>6.33</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -631,7 +631,7 @@
         <v>5.29</v>
       </c>
       <c r="G9" t="n">
-        <v>6.1</v>
+        <v>6.27</v>
       </c>
       <c r="H9" t="s">
         <v>13</v>
@@ -640,22 +640,22 @@
     <row r="10">
       <c r="A10"/>
       <c r="B10" t="n">
-        <v>4000.03</v>
+        <v>4000</v>
       </c>
       <c r="C10" t="n">
-        <v>4400.97</v>
+        <v>4398.75</v>
       </c>
       <c r="D10" t="n">
-        <v>7976.44</v>
+        <v>7976.39</v>
       </c>
       <c r="E10" t="n">
-        <v>7894.66</v>
+        <v>7898.23</v>
       </c>
       <c r="F10" t="n">
-        <v>12083.2</v>
+        <v>12079.54</v>
       </c>
       <c r="G10" t="n">
-        <v>12999.97</v>
+        <v>12999.99</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
@@ -667,16 +667,16 @@
         <v>4000</v>
       </c>
       <c r="C11" t="n">
-        <v>4399.66</v>
+        <v>4399.27</v>
       </c>
       <c r="D11" t="n">
-        <v>7977.19</v>
+        <v>7978.32</v>
       </c>
       <c r="E11" t="n">
-        <v>7900.23</v>
+        <v>7900.75</v>
       </c>
       <c r="F11" t="n">
-        <v>12080.98</v>
+        <v>12082.2</v>
       </c>
       <c r="G11" t="n">
         <v>13000</v>
@@ -787,10 +787,10 @@
         <v>100</v>
       </c>
       <c r="C16" t="n">
-        <v>101.01</v>
+        <v>101</v>
       </c>
       <c r="D16" t="n">
-        <v>119.99</v>
+        <v>120</v>
       </c>
       <c r="E16" t="n">
         <v>120</v>
@@ -814,13 +814,13 @@
         <v>101</v>
       </c>
       <c r="D17" t="n">
-        <v>120</v>
+        <v>119.99</v>
       </c>
       <c r="E17" t="n">
         <v>119.99</v>
       </c>
       <c r="F17" t="n">
-        <v>139.01</v>
+        <v>139</v>
       </c>
       <c r="G17" t="n">
         <v>140</v>
@@ -844,7 +844,7 @@
         <v>0.25</v>
       </c>
       <c r="F18" t="n">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="G18" t="n">
         <v>0.35</v>
@@ -859,7 +859,7 @@
         <v>0.15</v>
       </c>
       <c r="C19" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="D19" t="n">
         <v>0.25</v>
@@ -868,7 +868,7 @@
         <v>0.25</v>
       </c>
       <c r="F19" t="n">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="G19" t="n">
         <v>0.35</v>
@@ -928,22 +928,22 @@
     <row r="22">
       <c r="A22"/>
       <c r="B22" t="n">
-        <v>8103.86</v>
+        <v>7983.03</v>
       </c>
       <c r="C22" t="n">
-        <v>9306.17</v>
+        <v>9307.61</v>
       </c>
       <c r="D22" t="n">
-        <v>11633.46</v>
+        <v>11632.73</v>
       </c>
       <c r="E22" t="n">
-        <v>11581.15</v>
+        <v>11580.81</v>
       </c>
       <c r="F22" t="n">
-        <v>14314.03</v>
+        <v>14310.4</v>
       </c>
       <c r="G22" t="n">
-        <v>16714.51</v>
+        <v>16765.13</v>
       </c>
       <c r="H22" t="s">
         <v>21</v>
@@ -952,22 +952,22 @@
     <row r="23">
       <c r="A23"/>
       <c r="B23" t="n">
-        <v>9928.79</v>
+        <v>9761.47</v>
       </c>
       <c r="C23" t="n">
-        <v>12839.56</v>
+        <v>12837.3</v>
       </c>
       <c r="D23" t="n">
-        <v>16568.59</v>
+        <v>16568.43</v>
       </c>
       <c r="E23" t="n">
-        <v>16462.88</v>
+        <v>16461.64</v>
       </c>
       <c r="F23" t="n">
-        <v>20925.14</v>
+        <v>20920.88</v>
       </c>
       <c r="G23" t="n">
-        <v>26893.58</v>
+        <v>27570.41</v>
       </c>
       <c r="H23" t="s">
         <v>22</v>
@@ -976,7 +976,7 @@
     <row r="24">
       <c r="A24"/>
       <c r="B24" t="n">
-        <v>0.95</v>
+        <v>0.88</v>
       </c>
       <c r="C24" t="n">
         <v>1.37</v>
@@ -991,7 +991,7 @@
         <v>4.27</v>
       </c>
       <c r="G24" t="n">
-        <v>6.5</v>
+        <v>6.91</v>
       </c>
       <c r="H24" t="s">
         <v>23</v>

</xml_diff>